<commit_message>
this is my latest commit
</commit_message>
<xml_diff>
--- a/KeywordFiles/346780.xlsx
+++ b/KeywordFiles/346780.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="51">
   <si>
     <t>Test Case Id</t>
   </si>
@@ -77,9 +77,6 @@
     <t>precondition</t>
   </si>
   <si>
-    <t>Trauma Status Upgrade</t>
-  </si>
-  <si>
     <t>Level 4 Medical</t>
   </si>
   <si>
@@ -98,15 +95,9 @@
     <t>PriorityModalWndConf</t>
   </si>
   <si>
-    <t>Level 1 Medical</t>
-  </si>
-  <si>
     <t>FnCreateUct</t>
   </si>
   <si>
-    <t>7000 Lusk Bl</t>
-  </si>
-  <si>
     <t xml:space="preserve">Additional Information </t>
   </si>
   <si>
@@ -137,9 +128,6 @@
     <t>Pt Condition Upgrade</t>
   </si>
   <si>
-    <t>Gunshot Wound (L3)</t>
-  </si>
-  <si>
     <t>SetDefInMSI</t>
   </si>
   <si>
@@ -171,13 +159,31 @@
   </si>
   <si>
     <t>Test Memo 2</t>
+  </si>
+  <si>
+    <t>8583 AERO DR</t>
+  </si>
+  <si>
+    <t>Level 2 Medical</t>
+  </si>
+  <si>
+    <t>FnVerifyPriorityChangeFromDb</t>
+  </si>
+  <si>
+    <t>odtincident(0)</t>
+  </si>
+  <si>
+    <t>GetIncidentdetailstoodt</t>
+  </si>
+  <si>
+    <t>Breathing Problem (L3)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -235,14 +241,6 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="9"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -259,7 +257,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC000"/>
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -301,10 +299,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -619,10 +619,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S66"/>
+  <dimension ref="A1:S69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E41" sqref="E41"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -638,7 +638,7 @@
     <col min="9" max="9" width="38.42578125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="30.7109375" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="28.28515625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="75.5703125" customWidth="1"/>
     <col min="13" max="13" width="13.85546875" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="15.5703125" bestFit="1" customWidth="1"/>
     <col min="15" max="16" width="11.28515625" bestFit="1" customWidth="1"/>
@@ -710,45 +710,44 @@
         <v>1</v>
       </c>
       <c r="D2" s="12" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E2" s="12"/>
       <c r="F2" s="12"/>
       <c r="G2" s="12"/>
       <c r="H2" s="12"/>
       <c r="I2" s="12" t="s">
-        <v>26</v>
+        <v>45</v>
       </c>
       <c r="J2" s="12" t="s">
-        <v>37</v>
+        <v>50</v>
       </c>
       <c r="K2" s="12" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
     </row>
     <row r="3" spans="1:19" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="18">
-        <v>346780</v>
-      </c>
-      <c r="B3" s="18">
+      <c r="A3" s="12">
+        <v>346780</v>
+      </c>
+      <c r="B3" s="12">
         <v>2</v>
       </c>
-      <c r="C3" s="18">
+      <c r="C3" s="12">
         <v>2</v>
       </c>
-      <c r="D3" s="21" t="s">
-        <v>44</v>
-      </c>
-      <c r="E3" s="18"/>
-      <c r="F3" s="18"/>
-      <c r="G3" s="18"/>
-      <c r="H3" s="18"/>
-      <c r="I3" s="18">
-        <v>10000</v>
-      </c>
-      <c r="J3" s="18"/>
-      <c r="K3" s="18"/>
-      <c r="L3" s="19"/>
+      <c r="D3" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="E3" s="12"/>
+      <c r="F3" s="12"/>
+      <c r="G3" s="12"/>
+      <c r="H3" s="12"/>
+      <c r="I3" s="12">
+        <v>2000</v>
+      </c>
+      <c r="J3" s="12"/>
+      <c r="K3" s="12"/>
     </row>
     <row r="4" spans="1:19" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="12">
@@ -761,14 +760,14 @@
         <v>3</v>
       </c>
       <c r="D4" s="12" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E4" s="12"/>
       <c r="F4" s="12"/>
       <c r="G4" s="12"/>
       <c r="H4" s="12"/>
       <c r="I4" s="12" t="s">
-        <v>24</v>
+        <v>46</v>
       </c>
       <c r="J4" s="12"/>
       <c r="K4" s="12"/>
@@ -784,17 +783,17 @@
         <v>4</v>
       </c>
       <c r="D5" s="12" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E5" s="12"/>
       <c r="F5" s="12"/>
       <c r="G5" s="12"/>
       <c r="H5" s="12"/>
       <c r="I5" s="12" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="J5" s="12" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="K5" s="12"/>
     </row>
@@ -809,7 +808,7 @@
         <v>5</v>
       </c>
       <c r="D6" s="12" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E6" s="12"/>
       <c r="F6" s="12"/>
@@ -819,7 +818,7 @@
       <c r="J6" s="12"/>
       <c r="K6" s="12"/>
     </row>
-    <row r="7" spans="1:19" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:19" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="12">
         <v>346780</v>
       </c>
@@ -830,25 +829,17 @@
         <v>6</v>
       </c>
       <c r="D7" s="12" t="s">
-        <v>22</v>
+        <v>36</v>
       </c>
       <c r="E7" s="12"/>
       <c r="F7" s="12"/>
       <c r="G7" s="12"/>
       <c r="H7" s="12"/>
       <c r="I7" s="12" t="s">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="J7" s="12"/>
       <c r="K7" s="12"/>
-      <c r="L7" s="11"/>
-      <c r="M7" s="11"/>
-      <c r="N7" s="11"/>
-      <c r="O7" s="11"/>
-      <c r="P7" s="11"/>
-      <c r="Q7" s="11"/>
-      <c r="R7" s="11"/>
-      <c r="S7" s="11"/>
     </row>
     <row r="8" spans="1:19" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="12">
@@ -861,18 +852,14 @@
         <v>7</v>
       </c>
       <c r="D8" s="12" t="s">
-        <v>20</v>
+        <v>49</v>
       </c>
       <c r="E8" s="12"/>
       <c r="F8" s="12"/>
       <c r="G8" s="12"/>
       <c r="H8" s="12"/>
-      <c r="I8" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="J8" s="12" t="s">
-        <v>27</v>
-      </c>
+      <c r="I8" s="12"/>
+      <c r="J8" s="12"/>
       <c r="K8" s="12"/>
     </row>
     <row r="9" spans="1:19" s="11" customFormat="1" x14ac:dyDescent="0.25">
@@ -886,18 +873,26 @@
         <v>8</v>
       </c>
       <c r="D9" s="12" t="s">
-        <v>23</v>
+        <v>47</v>
       </c>
       <c r="E9" s="12"/>
       <c r="F9" s="12"/>
       <c r="G9" s="12"/>
       <c r="H9" s="12"/>
-      <c r="I9" s="12"/>
-      <c r="J9" s="12"/>
-      <c r="K9" s="12"/>
-    </row>
-    <row r="10" spans="1:19" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="12">
+      <c r="I9" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="J9" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="K9" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="L9" s="12"/>
+      <c r="M9" s="12"/>
+    </row>
+    <row r="10" spans="1:19" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="20">
         <v>346780</v>
       </c>
       <c r="B10" s="12">
@@ -906,21 +901,22 @@
       <c r="C10" s="12">
         <v>9</v>
       </c>
-      <c r="D10" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="E10" s="12"/>
-      <c r="F10" s="12"/>
-      <c r="G10" s="12"/>
-      <c r="H10" s="12"/>
-      <c r="I10" s="12" t="s">
-        <v>29</v>
-      </c>
-      <c r="J10" s="12"/>
-      <c r="K10" s="12"/>
-      <c r="L10" s="17"/>
-    </row>
-    <row r="11" spans="1:19" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D10" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="E10" s="20"/>
+      <c r="F10" s="20"/>
+      <c r="G10" s="20"/>
+      <c r="H10" s="20"/>
+      <c r="I10" s="20">
+        <v>990000</v>
+      </c>
+      <c r="J10" s="20"/>
+      <c r="K10" s="20"/>
+      <c r="L10" s="20"/>
+      <c r="M10" s="20"/>
+    </row>
+    <row r="11" spans="1:19" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="12">
         <v>346780</v>
       </c>
@@ -931,21 +927,27 @@
         <v>10</v>
       </c>
       <c r="D11" s="12" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E11" s="12"/>
       <c r="F11" s="12"/>
       <c r="G11" s="12"/>
       <c r="H11" s="12"/>
       <c r="I11" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="J11" s="12" t="s">
-        <v>30</v>
-      </c>
+        <v>25</v>
+      </c>
+      <c r="J11" s="12"/>
       <c r="K11" s="12"/>
-    </row>
-    <row r="12" spans="1:19" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="L11" s="11"/>
+      <c r="M11" s="11"/>
+      <c r="N11" s="11"/>
+      <c r="O11" s="11"/>
+      <c r="P11" s="11"/>
+      <c r="Q11" s="11"/>
+      <c r="R11" s="11"/>
+      <c r="S11" s="11"/>
+    </row>
+    <row r="12" spans="1:19" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="12">
         <v>346780</v>
       </c>
@@ -956,25 +958,21 @@
         <v>11</v>
       </c>
       <c r="D12" s="12" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="E12" s="12"/>
       <c r="F12" s="12"/>
       <c r="G12" s="12"/>
       <c r="H12" s="12"/>
-      <c r="I12" s="12"/>
-      <c r="J12" s="12"/>
+      <c r="I12" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="J12" s="12" t="s">
+        <v>24</v>
+      </c>
       <c r="K12" s="12"/>
-      <c r="L12" s="11"/>
-      <c r="M12" s="11"/>
-      <c r="N12" s="11"/>
-      <c r="O12" s="11"/>
-      <c r="P12" s="11"/>
-      <c r="Q12" s="11"/>
-      <c r="R12" s="11"/>
-      <c r="S12" s="11"/>
-    </row>
-    <row r="13" spans="1:19" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:19" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="12">
         <v>346780</v>
       </c>
@@ -991,21 +989,11 @@
       <c r="F13" s="12"/>
       <c r="G13" s="12"/>
       <c r="H13" s="12"/>
-      <c r="I13" s="12" t="s">
-        <v>18</v>
-      </c>
+      <c r="I13" s="12"/>
       <c r="J13" s="12"/>
       <c r="K13" s="12"/>
-      <c r="L13" s="11"/>
-      <c r="M13" s="11"/>
-      <c r="N13" s="11"/>
-      <c r="O13" s="11"/>
-      <c r="P13" s="11"/>
-      <c r="Q13" s="11"/>
-      <c r="R13" s="11"/>
-      <c r="S13" s="11"/>
-    </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:19" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="12">
         <v>346780</v>
       </c>
@@ -1016,29 +1004,20 @@
         <v>13</v>
       </c>
       <c r="D14" s="12" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E14" s="12"/>
       <c r="F14" s="12"/>
       <c r="G14" s="12"/>
       <c r="H14" s="12"/>
       <c r="I14" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="J14" s="12" t="s">
-        <v>36</v>
-      </c>
+        <v>26</v>
+      </c>
+      <c r="J14" s="12"/>
       <c r="K14" s="12"/>
-      <c r="L14" s="11"/>
-      <c r="M14" s="11"/>
-      <c r="N14" s="11"/>
-      <c r="O14" s="11"/>
-      <c r="P14" s="11"/>
-      <c r="Q14" s="11"/>
-      <c r="R14" s="11"/>
-      <c r="S14" s="11"/>
-    </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="L14" s="17"/>
+    </row>
+    <row r="15" spans="1:19" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="12">
         <v>346780</v>
       </c>
@@ -1049,25 +1028,21 @@
         <v>14</v>
       </c>
       <c r="D15" s="12" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="E15" s="12"/>
       <c r="F15" s="12"/>
       <c r="G15" s="12"/>
       <c r="H15" s="12"/>
-      <c r="I15" s="12"/>
-      <c r="J15" s="12"/>
+      <c r="I15" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="J15" s="12" t="s">
+        <v>27</v>
+      </c>
       <c r="K15" s="12"/>
-      <c r="L15" s="11"/>
-      <c r="M15" s="11"/>
-      <c r="N15" s="11"/>
-      <c r="O15" s="11"/>
-      <c r="P15" s="11"/>
-      <c r="Q15" s="11"/>
-      <c r="R15" s="11"/>
-      <c r="S15" s="11"/>
-    </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:19" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="12">
         <v>346780</v>
       </c>
@@ -1084,9 +1059,7 @@
       <c r="F16" s="12"/>
       <c r="G16" s="12"/>
       <c r="H16" s="12"/>
-      <c r="I16" s="12" t="s">
-        <v>31</v>
-      </c>
+      <c r="I16" s="12"/>
       <c r="J16" s="12"/>
       <c r="K16" s="12"/>
       <c r="L16" s="11"/>
@@ -1098,7 +1071,7 @@
       <c r="R16" s="11"/>
       <c r="S16" s="11"/>
     </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:19" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="12">
         <v>346780</v>
       </c>
@@ -1109,18 +1082,16 @@
         <v>16</v>
       </c>
       <c r="D17" s="12" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E17" s="12"/>
       <c r="F17" s="12"/>
       <c r="G17" s="12"/>
       <c r="H17" s="12"/>
       <c r="I17" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="J17" s="12" t="s">
-        <v>19</v>
-      </c>
+        <v>17</v>
+      </c>
+      <c r="J17" s="12"/>
       <c r="K17" s="12"/>
       <c r="L17" s="11"/>
       <c r="M17" s="11"/>
@@ -1142,14 +1113,18 @@
         <v>17</v>
       </c>
       <c r="D18" s="12" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="E18" s="12"/>
       <c r="F18" s="12"/>
       <c r="G18" s="12"/>
       <c r="H18" s="12"/>
-      <c r="I18" s="12"/>
-      <c r="J18" s="12"/>
+      <c r="I18" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="J18" s="12" t="s">
+        <v>33</v>
+      </c>
       <c r="K18" s="12"/>
       <c r="L18" s="11"/>
       <c r="M18" s="11"/>
@@ -1177,18 +1152,17 @@
       <c r="F19" s="12"/>
       <c r="G19" s="12"/>
       <c r="H19" s="12"/>
-      <c r="I19" s="12" t="s">
-        <v>35</v>
-      </c>
+      <c r="I19" s="12"/>
       <c r="J19" s="12"/>
       <c r="K19" s="12"/>
-      <c r="L19" s="1"/>
-      <c r="M19" s="1"/>
-      <c r="N19" s="1"/>
-      <c r="O19" s="1"/>
-      <c r="P19" s="1"/>
-      <c r="Q19" s="1"/>
-      <c r="R19" s="1"/>
+      <c r="L19" s="11"/>
+      <c r="M19" s="11"/>
+      <c r="N19" s="11"/>
+      <c r="O19" s="11"/>
+      <c r="P19" s="11"/>
+      <c r="Q19" s="11"/>
+      <c r="R19" s="11"/>
+      <c r="S19" s="11"/>
     </row>
     <row r="20" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A20" s="12">
@@ -1201,26 +1175,25 @@
         <v>19</v>
       </c>
       <c r="D20" s="12" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E20" s="12"/>
       <c r="F20" s="12"/>
       <c r="G20" s="12"/>
       <c r="H20" s="12"/>
       <c r="I20" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="J20" s="12" t="s">
-        <v>32</v>
-      </c>
+        <v>28</v>
+      </c>
+      <c r="J20" s="12"/>
       <c r="K20" s="12"/>
-      <c r="L20" s="1"/>
-      <c r="M20" s="1"/>
-      <c r="N20" s="1"/>
-      <c r="O20" s="1"/>
-      <c r="P20" s="1"/>
-      <c r="Q20" s="1"/>
-      <c r="R20" s="1"/>
+      <c r="L20" s="11"/>
+      <c r="M20" s="11"/>
+      <c r="N20" s="11"/>
+      <c r="O20" s="11"/>
+      <c r="P20" s="11"/>
+      <c r="Q20" s="11"/>
+      <c r="R20" s="11"/>
+      <c r="S20" s="11"/>
     </row>
     <row r="21" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A21" s="12">
@@ -1233,22 +1206,27 @@
         <v>20</v>
       </c>
       <c r="D21" s="12" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="E21" s="12"/>
       <c r="F21" s="12"/>
       <c r="G21" s="12"/>
       <c r="H21" s="12"/>
-      <c r="I21" s="12"/>
-      <c r="J21" s="12"/>
+      <c r="I21" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="J21" s="12" t="s">
+        <v>18</v>
+      </c>
       <c r="K21" s="12"/>
-      <c r="L21" s="1"/>
-      <c r="M21" s="1"/>
-      <c r="N21" s="1"/>
-      <c r="O21" s="1"/>
-      <c r="P21" s="1"/>
-      <c r="Q21" s="1"/>
-      <c r="R21" s="1"/>
+      <c r="L21" s="11"/>
+      <c r="M21" s="11"/>
+      <c r="N21" s="11"/>
+      <c r="O21" s="11"/>
+      <c r="P21" s="11"/>
+      <c r="Q21" s="11"/>
+      <c r="R21" s="11"/>
+      <c r="S21" s="11"/>
     </row>
     <row r="22" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A22" s="12">
@@ -1267,18 +1245,17 @@
       <c r="F22" s="12"/>
       <c r="G22" s="12"/>
       <c r="H22" s="12"/>
-      <c r="I22" s="12" t="s">
-        <v>34</v>
-      </c>
+      <c r="I22" s="12"/>
       <c r="J22" s="12"/>
       <c r="K22" s="12"/>
-      <c r="L22" s="1"/>
-      <c r="M22" s="1"/>
-      <c r="N22" s="1"/>
-      <c r="O22" s="1"/>
-      <c r="P22" s="1"/>
-      <c r="Q22" s="1"/>
-      <c r="R22" s="1"/>
+      <c r="L22" s="11"/>
+      <c r="M22" s="11"/>
+      <c r="N22" s="11"/>
+      <c r="O22" s="11"/>
+      <c r="P22" s="11"/>
+      <c r="Q22" s="11"/>
+      <c r="R22" s="11"/>
+      <c r="S22" s="11"/>
     </row>
     <row r="23" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A23" s="12">
@@ -1291,19 +1268,17 @@
         <v>22</v>
       </c>
       <c r="D23" s="12" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E23" s="12"/>
       <c r="F23" s="12"/>
       <c r="G23" s="12"/>
       <c r="H23" s="12"/>
       <c r="I23" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="J23" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="K23" s="13"/>
+        <v>32</v>
+      </c>
+      <c r="J23" s="12"/>
+      <c r="K23" s="12"/>
       <c r="L23" s="1"/>
       <c r="M23" s="1"/>
       <c r="N23" s="1"/>
@@ -1323,14 +1298,18 @@
         <v>23</v>
       </c>
       <c r="D24" s="12" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="E24" s="12"/>
       <c r="F24" s="12"/>
       <c r="G24" s="12"/>
       <c r="H24" s="12"/>
-      <c r="I24" s="12"/>
-      <c r="J24" s="12"/>
+      <c r="I24" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="J24" s="12" t="s">
+        <v>29</v>
+      </c>
       <c r="K24" s="12"/>
       <c r="L24" s="1"/>
       <c r="M24" s="1"/>
@@ -1340,7 +1319,7 @@
       <c r="Q24" s="1"/>
       <c r="R24" s="1"/>
     </row>
-    <row r="25" spans="1:19" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A25" s="12">
         <v>346780</v>
       </c>
@@ -1357,12 +1336,10 @@
       <c r="F25" s="12"/>
       <c r="G25" s="12"/>
       <c r="H25" s="12"/>
-      <c r="I25" s="12" t="s">
-        <v>18</v>
-      </c>
+      <c r="I25" s="12"/>
       <c r="J25" s="12"/>
       <c r="K25" s="12"/>
-      <c r="L25" s="10"/>
+      <c r="L25" s="1"/>
       <c r="M25" s="1"/>
       <c r="N25" s="1"/>
       <c r="O25" s="1"/>
@@ -1370,7 +1347,7 @@
       <c r="Q25" s="1"/>
       <c r="R25" s="1"/>
     </row>
-    <row r="26" spans="1:19" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A26" s="12">
         <v>346780</v>
       </c>
@@ -1381,20 +1358,18 @@
         <v>25</v>
       </c>
       <c r="D26" s="12" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E26" s="12"/>
       <c r="F26" s="12"/>
       <c r="G26" s="12"/>
       <c r="H26" s="12"/>
       <c r="I26" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="J26" s="12" t="s">
-        <v>33</v>
-      </c>
+        <v>31</v>
+      </c>
+      <c r="J26" s="12"/>
       <c r="K26" s="12"/>
-      <c r="L26" s="9"/>
+      <c r="L26" s="1"/>
       <c r="M26" s="1"/>
       <c r="N26" s="1"/>
       <c r="O26" s="1"/>
@@ -1402,7 +1377,7 @@
       <c r="Q26" s="1"/>
       <c r="R26" s="1"/>
     </row>
-    <row r="27" spans="1:19" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A27" s="12">
         <v>346780</v>
       </c>
@@ -1413,16 +1388,20 @@
         <v>26</v>
       </c>
       <c r="D27" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="E27" s="14"/>
-      <c r="F27" s="14"/>
-      <c r="G27" s="14"/>
-      <c r="H27" s="14"/>
-      <c r="I27" s="12"/>
-      <c r="J27" s="14"/>
-      <c r="K27" s="12"/>
-      <c r="L27" s="10"/>
+        <v>19</v>
+      </c>
+      <c r="E27" s="12"/>
+      <c r="F27" s="12"/>
+      <c r="G27" s="12"/>
+      <c r="H27" s="12"/>
+      <c r="I27" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="J27" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="K27" s="13"/>
+      <c r="L27" s="1"/>
       <c r="M27" s="1"/>
       <c r="N27" s="1"/>
       <c r="O27" s="1"/>
@@ -1441,15 +1420,13 @@
         <v>27</v>
       </c>
       <c r="D28" s="12" t="s">
-        <v>40</v>
+        <v>22</v>
       </c>
       <c r="E28" s="12"/>
       <c r="F28" s="12"/>
       <c r="G28" s="12"/>
       <c r="H28" s="12"/>
-      <c r="I28" s="12" t="s">
-        <v>41</v>
-      </c>
+      <c r="I28" s="12"/>
       <c r="J28" s="12"/>
       <c r="K28" s="12"/>
       <c r="L28" s="1"/>
@@ -1460,7 +1437,7 @@
       <c r="Q28" s="1"/>
       <c r="R28" s="1"/>
     </row>
-    <row r="29" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:19" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="12">
         <v>346780</v>
       </c>
@@ -1471,16 +1448,18 @@
         <v>28</v>
       </c>
       <c r="D29" s="12" t="s">
-        <v>38</v>
+        <v>21</v>
       </c>
       <c r="E29" s="12"/>
       <c r="F29" s="12"/>
       <c r="G29" s="12"/>
       <c r="H29" s="12"/>
-      <c r="I29" s="12"/>
+      <c r="I29" s="12" t="s">
+        <v>17</v>
+      </c>
       <c r="J29" s="12"/>
       <c r="K29" s="12"/>
-      <c r="L29" s="1"/>
+      <c r="L29" s="10"/>
       <c r="M29" s="1"/>
       <c r="N29" s="1"/>
       <c r="O29" s="1"/>
@@ -1488,7 +1467,7 @@
       <c r="Q29" s="1"/>
       <c r="R29" s="1"/>
     </row>
-    <row r="30" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:19" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="12">
         <v>346780</v>
       </c>
@@ -1499,39 +1478,54 @@
         <v>29</v>
       </c>
       <c r="D30" s="12" t="s">
-        <v>42</v>
+        <v>19</v>
       </c>
       <c r="E30" s="12"/>
       <c r="F30" s="12"/>
       <c r="G30" s="12"/>
       <c r="H30" s="12"/>
-      <c r="I30" s="15"/>
-      <c r="J30" s="15"/>
+      <c r="I30" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="J30" s="12" t="s">
+        <v>30</v>
+      </c>
       <c r="K30" s="12"/>
-    </row>
-    <row r="31" spans="1:19" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="18">
-        <v>346780</v>
-      </c>
-      <c r="B31" s="18">
+      <c r="L30" s="9"/>
+      <c r="M30" s="1"/>
+      <c r="N30" s="1"/>
+      <c r="O30" s="1"/>
+      <c r="P30" s="1"/>
+      <c r="Q30" s="1"/>
+      <c r="R30" s="1"/>
+    </row>
+    <row r="31" spans="1:19" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="12">
+        <v>346780</v>
+      </c>
+      <c r="B31" s="12">
         <v>30</v>
       </c>
-      <c r="C31" s="18">
+      <c r="C31" s="12">
         <v>30</v>
       </c>
-      <c r="D31" s="21" t="s">
-        <v>44</v>
-      </c>
-      <c r="E31" s="18"/>
-      <c r="F31" s="18"/>
-      <c r="G31" s="18"/>
-      <c r="H31" s="18"/>
-      <c r="I31" s="18">
-        <v>10000</v>
-      </c>
-      <c r="J31" s="18"/>
-      <c r="K31" s="18"/>
-      <c r="L31" s="19"/>
+      <c r="D31" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="E31" s="14"/>
+      <c r="F31" s="14"/>
+      <c r="G31" s="14"/>
+      <c r="H31" s="14"/>
+      <c r="I31" s="12"/>
+      <c r="J31" s="14"/>
+      <c r="K31" s="12"/>
+      <c r="L31" s="10"/>
+      <c r="M31" s="1"/>
+      <c r="N31" s="1"/>
+      <c r="O31" s="1"/>
+      <c r="P31" s="1"/>
+      <c r="Q31" s="1"/>
+      <c r="R31" s="1"/>
     </row>
     <row r="32" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A32" s="12">
@@ -1544,17 +1538,24 @@
         <v>31</v>
       </c>
       <c r="D32" s="12" t="s">
-        <v>22</v>
+        <v>36</v>
       </c>
       <c r="E32" s="12"/>
-      <c r="F32" s="14"/>
-      <c r="G32" s="14"/>
-      <c r="H32" s="14"/>
+      <c r="F32" s="12"/>
+      <c r="G32" s="12"/>
+      <c r="H32" s="12"/>
       <c r="I32" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="J32" s="14"/>
+        <v>37</v>
+      </c>
+      <c r="J32" s="12"/>
       <c r="K32" s="12"/>
+      <c r="L32" s="1"/>
+      <c r="M32" s="1"/>
+      <c r="N32" s="1"/>
+      <c r="O32" s="1"/>
+      <c r="P32" s="1"/>
+      <c r="Q32" s="1"/>
+      <c r="R32" s="1"/>
     </row>
     <row r="33" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A33" s="12">
@@ -1567,18 +1568,22 @@
         <v>32</v>
       </c>
       <c r="D33" s="12" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="E33" s="12"/>
-      <c r="F33" s="14"/>
-      <c r="G33" s="14"/>
-      <c r="H33" s="14"/>
-      <c r="I33" s="14" t="s">
-        <v>31</v>
-      </c>
+      <c r="F33" s="12"/>
+      <c r="G33" s="12"/>
+      <c r="H33" s="12"/>
+      <c r="I33" s="12"/>
       <c r="J33" s="12"/>
       <c r="K33" s="12"/>
+      <c r="L33" s="1"/>
+      <c r="M33" s="1"/>
+      <c r="N33" s="1"/>
+      <c r="O33" s="1"/>
       <c r="P33" s="1"/>
+      <c r="Q33" s="1"/>
+      <c r="R33" s="1"/>
     </row>
     <row r="34" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A34" s="12">
@@ -1591,21 +1596,17 @@
         <v>33</v>
       </c>
       <c r="D34" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="E34" s="16"/>
-      <c r="F34" s="16"/>
-      <c r="G34" s="16"/>
-      <c r="H34" s="16"/>
-      <c r="I34" s="12" t="s">
-        <v>39</v>
-      </c>
-      <c r="J34" s="14"/>
+        <v>38</v>
+      </c>
+      <c r="E34" s="12"/>
+      <c r="F34" s="12"/>
+      <c r="G34" s="12"/>
+      <c r="H34" s="12"/>
+      <c r="I34" s="15"/>
+      <c r="J34" s="15"/>
       <c r="K34" s="12"/>
-      <c r="L34" s="4"/>
-      <c r="P34" s="1"/>
-    </row>
-    <row r="35" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="35" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A35" s="12">
         <v>346780</v>
       </c>
@@ -1616,19 +1617,17 @@
         <v>34</v>
       </c>
       <c r="D35" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="E35" s="14"/>
+        <v>21</v>
+      </c>
+      <c r="E35" s="12"/>
       <c r="F35" s="14"/>
       <c r="G35" s="14"/>
       <c r="H35" s="14"/>
       <c r="I35" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="J35" s="20"/>
+        <v>17</v>
+      </c>
+      <c r="J35" s="14"/>
       <c r="K35" s="12"/>
-      <c r="L35" s="4"/>
-      <c r="P35" s="1"/>
     </row>
     <row r="36" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A36" s="12">
@@ -1641,20 +1640,18 @@
         <v>35</v>
       </c>
       <c r="D36" s="12" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E36" s="12"/>
       <c r="F36" s="14"/>
       <c r="G36" s="14"/>
       <c r="H36" s="14"/>
-      <c r="I36" s="12" t="s">
-        <v>45</v>
+      <c r="I36" s="14" t="s">
+        <v>28</v>
       </c>
       <c r="J36" s="12"/>
       <c r="K36" s="12"/>
-      <c r="L36" s="4"/>
-      <c r="Q36" s="1"/>
-      <c r="R36" s="1"/>
+      <c r="P36" s="1"/>
     </row>
     <row r="37" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A37" s="12">
@@ -1667,23 +1664,21 @@
         <v>36</v>
       </c>
       <c r="D37" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="E37" s="12"/>
-      <c r="F37" s="14"/>
-      <c r="G37" s="14"/>
-      <c r="H37" s="14"/>
-      <c r="I37" s="14" t="s">
-        <v>46</v>
+        <v>21</v>
+      </c>
+      <c r="E37" s="16"/>
+      <c r="F37" s="16"/>
+      <c r="G37" s="16"/>
+      <c r="H37" s="16"/>
+      <c r="I37" s="12" t="s">
+        <v>35</v>
       </c>
       <c r="J37" s="14"/>
       <c r="K37" s="12"/>
       <c r="L37" s="4"/>
       <c r="P37" s="1"/>
-      <c r="Q37" s="1"/>
-      <c r="R37" s="1"/>
-    </row>
-    <row r="38" spans="1:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="38" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="12">
         <v>346780</v>
       </c>
@@ -1694,21 +1689,19 @@
         <v>37</v>
       </c>
       <c r="D38" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="E38" s="16"/>
-      <c r="F38" s="16"/>
-      <c r="G38" s="16"/>
-      <c r="H38" s="16"/>
+        <v>21</v>
+      </c>
+      <c r="E38" s="14"/>
+      <c r="F38" s="14"/>
+      <c r="G38" s="14"/>
+      <c r="H38" s="14"/>
       <c r="I38" s="12" t="s">
-        <v>47</v>
-      </c>
-      <c r="J38" s="12"/>
+        <v>32</v>
+      </c>
+      <c r="J38" s="18"/>
       <c r="K38" s="12"/>
       <c r="L38" s="4"/>
       <c r="P38" s="1"/>
-      <c r="Q38" s="1"/>
-      <c r="R38" s="1"/>
     </row>
     <row r="39" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A39" s="12">
@@ -1721,17 +1714,18 @@
         <v>38</v>
       </c>
       <c r="D39" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="E39" s="14"/>
+        <v>21</v>
+      </c>
+      <c r="E39" s="12"/>
       <c r="F39" s="14"/>
       <c r="G39" s="14"/>
       <c r="H39" s="14"/>
       <c r="I39" s="12" t="s">
-        <v>35</v>
-      </c>
+        <v>41</v>
+      </c>
+      <c r="J39" s="12"/>
+      <c r="K39" s="12"/>
       <c r="L39" s="4"/>
-      <c r="P39" s="1"/>
       <c r="Q39" s="1"/>
       <c r="R39" s="1"/>
     </row>
@@ -1746,72 +1740,129 @@
         <v>39</v>
       </c>
       <c r="D40" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="I40" s="12" t="s">
-        <v>48</v>
-      </c>
+        <v>21</v>
+      </c>
+      <c r="E40" s="12"/>
+      <c r="F40" s="14"/>
+      <c r="G40" s="14"/>
+      <c r="H40" s="14"/>
+      <c r="I40" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="J40" s="14"/>
+      <c r="K40" s="12"/>
       <c r="L40" s="4"/>
       <c r="P40" s="1"/>
       <c r="Q40" s="1"/>
       <c r="R40" s="1"/>
     </row>
     <row r="41" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="D41" s="7"/>
-      <c r="E41" s="7"/>
-      <c r="F41" s="7"/>
-      <c r="G41" s="7"/>
-      <c r="H41" s="7"/>
-      <c r="I41" s="7"/>
-      <c r="J41" s="7"/>
-      <c r="K41" s="4"/>
+      <c r="A41" s="12">
+        <v>346780</v>
+      </c>
+      <c r="B41" s="12">
+        <v>40</v>
+      </c>
+      <c r="C41" s="12">
+        <v>40</v>
+      </c>
+      <c r="D41" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="E41" s="16"/>
+      <c r="F41" s="16"/>
+      <c r="G41" s="16"/>
+      <c r="H41" s="16"/>
+      <c r="I41" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="J41" s="12"/>
+      <c r="K41" s="12"/>
       <c r="L41" s="4"/>
+      <c r="P41" s="1"/>
       <c r="Q41" s="1"/>
       <c r="R41" s="1"/>
     </row>
     <row r="42" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="D42" s="7"/>
-      <c r="E42" s="7"/>
-      <c r="F42" s="7"/>
-      <c r="G42" s="7"/>
-      <c r="H42" s="7"/>
-      <c r="I42" s="7"/>
-      <c r="J42" s="7"/>
-      <c r="K42" s="4"/>
+      <c r="A42" s="12">
+        <v>346780</v>
+      </c>
+      <c r="B42" s="12">
+        <v>41</v>
+      </c>
+      <c r="C42" s="12">
+        <v>41</v>
+      </c>
+      <c r="D42" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="E42" s="14"/>
+      <c r="F42" s="14"/>
+      <c r="G42" s="14"/>
+      <c r="H42" s="14"/>
+      <c r="I42" s="12" t="s">
+        <v>32</v>
+      </c>
       <c r="L42" s="4"/>
+      <c r="P42" s="1"/>
       <c r="Q42" s="1"/>
       <c r="R42" s="1"/>
     </row>
     <row r="43" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="D43" s="7"/>
-      <c r="E43" s="7"/>
-      <c r="F43" s="7"/>
-      <c r="G43" s="7"/>
-      <c r="H43" s="7"/>
-      <c r="I43" s="7"/>
-      <c r="J43" s="7"/>
-      <c r="K43" s="4"/>
+      <c r="A43" s="12">
+        <v>346780</v>
+      </c>
+      <c r="B43" s="12">
+        <v>42</v>
+      </c>
+      <c r="C43" s="12">
+        <v>42</v>
+      </c>
+      <c r="D43" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="I43" s="12" t="s">
+        <v>44</v>
+      </c>
       <c r="L43" s="4"/>
+      <c r="P43" s="1"/>
       <c r="Q43" s="1"/>
       <c r="R43" s="1"/>
     </row>
     <row r="44" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="D44" s="7"/>
+      <c r="E44" s="7"/>
+      <c r="F44" s="7"/>
+      <c r="G44" s="7"/>
+      <c r="H44" s="7"/>
+      <c r="I44" s="7"/>
+      <c r="J44" s="7"/>
       <c r="K44" s="4"/>
-      <c r="L44" s="5"/>
+      <c r="L44" s="4"/>
       <c r="Q44" s="1"/>
       <c r="R44" s="1"/>
     </row>
     <row r="45" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="D45" s="7"/>
+      <c r="E45" s="7"/>
+      <c r="F45" s="7"/>
+      <c r="G45" s="7"/>
+      <c r="H45" s="7"/>
+      <c r="I45" s="7"/>
+      <c r="J45" s="7"/>
       <c r="K45" s="4"/>
-      <c r="L45" s="6"/>
-      <c r="M45" s="1"/>
-      <c r="N45" s="1"/>
-      <c r="O45" s="1"/>
-      <c r="P45" s="1"/>
+      <c r="L45" s="4"/>
       <c r="Q45" s="1"/>
       <c r="R45" s="1"/>
     </row>
     <row r="46" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="D46" s="7"/>
+      <c r="E46" s="7"/>
+      <c r="F46" s="7"/>
+      <c r="G46" s="7"/>
+      <c r="H46" s="7"/>
+      <c r="I46" s="7"/>
+      <c r="J46" s="7"/>
       <c r="K46" s="4"/>
       <c r="L46" s="4"/>
       <c r="Q46" s="1"/>
@@ -1819,78 +1870,101 @@
     </row>
     <row r="47" spans="1:18" x14ac:dyDescent="0.25">
       <c r="K47" s="4"/>
-      <c r="L47" s="7"/>
+      <c r="L47" s="5"/>
+      <c r="Q47" s="1"/>
+      <c r="R47" s="1"/>
     </row>
     <row r="48" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="K48" s="7"/>
-      <c r="L48" s="7"/>
-    </row>
-    <row r="49" spans="11:18" x14ac:dyDescent="0.25">
-      <c r="K49" s="7"/>
-      <c r="L49" s="7"/>
-      <c r="N49" s="1"/>
-    </row>
-    <row r="50" spans="11:18" x14ac:dyDescent="0.25">
-      <c r="K50" s="7"/>
+      <c r="K48" s="4"/>
+      <c r="L48" s="6"/>
+      <c r="M48" s="1"/>
+      <c r="N48" s="1"/>
+      <c r="O48" s="1"/>
+      <c r="P48" s="1"/>
+      <c r="Q48" s="1"/>
+      <c r="R48" s="1"/>
+    </row>
+    <row r="49" spans="4:18" x14ac:dyDescent="0.25">
+      <c r="D49" s="19"/>
+      <c r="K49" s="4"/>
+      <c r="L49" s="4"/>
+      <c r="Q49" s="1"/>
+      <c r="R49" s="1"/>
+    </row>
+    <row r="50" spans="4:18" x14ac:dyDescent="0.25">
+      <c r="K50" s="4"/>
       <c r="L50" s="7"/>
-      <c r="N50" s="1"/>
-    </row>
-    <row r="51" spans="11:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="51" spans="4:18" x14ac:dyDescent="0.25">
       <c r="K51" s="7"/>
       <c r="L51" s="7"/>
-      <c r="N51" s="1"/>
-    </row>
-    <row r="52" spans="11:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="52" spans="4:18" x14ac:dyDescent="0.25">
       <c r="K52" s="7"/>
       <c r="L52" s="7"/>
       <c r="N52" s="1"/>
     </row>
-    <row r="53" spans="11:18" x14ac:dyDescent="0.25">
+    <row r="53" spans="4:18" x14ac:dyDescent="0.25">
       <c r="K53" s="7"/>
       <c r="L53" s="7"/>
       <c r="N53" s="1"/>
     </row>
-    <row r="54" spans="11:18" x14ac:dyDescent="0.25">
+    <row r="54" spans="4:18" x14ac:dyDescent="0.25">
+      <c r="K54" s="7"/>
       <c r="L54" s="7"/>
       <c r="N54" s="1"/>
     </row>
-    <row r="55" spans="11:18" x14ac:dyDescent="0.25">
+    <row r="55" spans="4:18" x14ac:dyDescent="0.25">
+      <c r="K55" s="7"/>
       <c r="L55" s="7"/>
       <c r="N55" s="1"/>
     </row>
-    <row r="56" spans="11:18" x14ac:dyDescent="0.25">
+    <row r="56" spans="4:18" x14ac:dyDescent="0.25">
+      <c r="K56" s="7"/>
+      <c r="L56" s="7"/>
       <c r="N56" s="1"/>
     </row>
-    <row r="58" spans="11:18" x14ac:dyDescent="0.25">
-      <c r="M58" s="1"/>
-    </row>
-    <row r="59" spans="11:18" x14ac:dyDescent="0.25">
-      <c r="M59" s="4"/>
-      <c r="N59" s="4"/>
-    </row>
-    <row r="60" spans="11:18" x14ac:dyDescent="0.25">
-      <c r="M60" s="1"/>
-      <c r="N60" s="1"/>
-    </row>
-    <row r="61" spans="11:18" x14ac:dyDescent="0.25">
+    <row r="57" spans="4:18" x14ac:dyDescent="0.25">
+      <c r="L57" s="7"/>
+      <c r="N57" s="1"/>
+    </row>
+    <row r="58" spans="4:18" x14ac:dyDescent="0.25">
+      <c r="L58" s="7"/>
+      <c r="N58" s="1"/>
+    </row>
+    <row r="59" spans="4:18" x14ac:dyDescent="0.25">
+      <c r="N59" s="1"/>
+    </row>
+    <row r="61" spans="4:18" x14ac:dyDescent="0.25">
       <c r="M61" s="1"/>
-      <c r="R61" s="1"/>
-    </row>
-    <row r="62" spans="11:18" x14ac:dyDescent="0.25">
-      <c r="M62" s="1"/>
-      <c r="R62" s="1"/>
-    </row>
-    <row r="63" spans="11:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="62" spans="4:18" x14ac:dyDescent="0.25">
+      <c r="M62" s="4"/>
+      <c r="N62" s="4"/>
+    </row>
+    <row r="63" spans="4:18" x14ac:dyDescent="0.25">
       <c r="M63" s="1"/>
-    </row>
-    <row r="64" spans="11:18" x14ac:dyDescent="0.25">
+      <c r="N63" s="1"/>
+    </row>
+    <row r="64" spans="4:18" x14ac:dyDescent="0.25">
       <c r="M64" s="1"/>
-    </row>
-    <row r="65" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="R64" s="1"/>
+    </row>
+    <row r="65" spans="13:18" x14ac:dyDescent="0.25">
       <c r="M65" s="1"/>
-    </row>
-    <row r="66" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="R65" s="1"/>
+    </row>
+    <row r="66" spans="13:18" x14ac:dyDescent="0.25">
       <c r="M66" s="1"/>
+    </row>
+    <row r="67" spans="13:18" x14ac:dyDescent="0.25">
+      <c r="M67" s="1"/>
+    </row>
+    <row r="68" spans="13:18" x14ac:dyDescent="0.25">
+      <c r="M68" s="1"/>
+    </row>
+    <row r="69" spans="13:18" x14ac:dyDescent="0.25">
+      <c r="M69" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>